<commit_message>
prmgs as on 05.08.24
</commit_message>
<xml_diff>
--- a/AshokIT_3/DataFiles/DataFile.xlsx
+++ b/AshokIT_3/DataFiles/DataFile.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\git\AshokITTestingTraining\AshokIT_3\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470D5B51-FBA0-4DD8-AA2A-87D9C51E2EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8BA565-27B1-4F51-925E-29A140014E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -376,7 +376,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>